<commit_message>
Added graphs to the data collected
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Output/Average data of all Scenario Trials.xlsx
+++ b/Assets/Scripts/Output/Average data of all Scenario Trials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nevada-my.sharepoint.com/personal/yashs_unr_edu/Documents/UNR Classes Stuff/School Year 2019-2020/Spring 2020/CPE 400 Class Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashs\Documents\GitHub\CPE400-UAV-Group-Project\Assets\Scripts\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="8_{2DB49026-B9D4-4477-B076-97008630C9DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CDB89CC1-257C-42AF-9448-DECE563A6153}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B918C740-C2A8-4FA2-9F62-9FA7242AF37D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{ABA30EFD-B823-4878-900F-504A818D0B68}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ABA30EFD-B823-4878-900F-504A818D0B68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
   <si>
     <t>Total Connected Users</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>Standard Deviation (Sample)</t>
+  </si>
+  <si>
+    <t>Standard Deviation (Population)</t>
   </si>
 </sst>
 </file>
@@ -132,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -146,14 +152,20 @@
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="33">
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -168,44 +180,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -225,7 +200,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -245,7 +220,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -265,7 +240,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -285,7 +260,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -305,7 +280,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -325,7 +300,347 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -368,247 +683,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -665,7 +740,64 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -695,18 +827,1039 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Users Served</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numLit>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numLit>
+            </c:plus>
+            <c:minus>
+              <c:numLit>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numLit>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet1!$G$2,Sheet1!$G$10,Sheet1!$G$18)</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>150.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>188.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E95B-449F-A40F-86EC54CB748B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inBase"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="770610832"/>
+        <c:axId val="770606896"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="770610832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Scenarios</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="770606896"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="770606896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Maximum Users Served</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="770610832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1409700</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE2516B3-FA6D-4353-AADC-D8D720889671}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{202BEFCF-82A0-4BE4-B772-B72FD7758A78}" name="Table1" displayName="Table1" ref="A1:G7" totalsRowShown="0" headerRowDxfId="0" dataDxfId="24">
-  <autoFilter ref="A1:G7" xr:uid="{C1D44CF6-C625-44C8-94E8-9E5C73B63796}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8CAE1FE0-D6C5-4AC2-BA98-471AB4002743}" name="Scenario 1" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{87065CE6-3999-4497-B27A-551AA2D4C37B}" name="Trail 1" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{357648BE-1398-4E85-B71D-C10734CE18E2}" name="Trial 2" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{032FD0EF-5291-46E4-A21D-7DA1C27D1558}" name="Trial 3" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{5E9CE060-472C-49E9-B08B-A553D82B749E}" name="Trial 4" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{442FB71F-1F35-41CB-AFBA-BFFFD19408D2}" name="Trial 5" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{71460663-C821-4F0D-A527-43417778D933}" name="Average" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{202BEFCF-82A0-4BE4-B772-B72FD7758A78}" name="Table1" displayName="Table1" ref="A1:I7" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+  <autoFilter ref="A1:I7" xr:uid="{C1D44CF6-C625-44C8-94E8-9E5C73B63796}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{8CAE1FE0-D6C5-4AC2-BA98-471AB4002743}" name="Scenario 1" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{87065CE6-3999-4497-B27A-551AA2D4C37B}" name="Trail 1" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{357648BE-1398-4E85-B71D-C10734CE18E2}" name="Trial 2" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{032FD0EF-5291-46E4-A21D-7DA1C27D1558}" name="Trial 3" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{5E9CE060-472C-49E9-B08B-A553D82B749E}" name="Trial 4" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{442FB71F-1F35-41CB-AFBA-BFFFD19408D2}" name="Trial 5" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{71460663-C821-4F0D-A527-43417778D933}" name="Average" dataDxfId="18">
       <calculatedColumnFormula>AVERAGE(Table1[[#This Row],[Trail 1]:[Trial 5]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{4F21015A-4791-4BEB-84C7-46BEEB65FA87}" name="Standard Deviation (Sample)" dataDxfId="17">
+      <calculatedColumnFormula>_xlfn.STDEV.S(Table1[[#This Row],[Trail 1]],Table1[[#This Row],[Trial 2]],Table1[[#This Row],[Trial 3]],Table1[[#This Row],[Trial 4]],Table1[[#This Row],[Trial 5]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{C869A0D5-EDB7-4F49-A730-D6041DB6619F}" name="Standard Deviation (Population)" dataDxfId="16">
+      <calculatedColumnFormula>_xlfn.STDEV.P(Table1[[#This Row],[Trail 1]],Table1[[#This Row],[Trial 2]],Table1[[#This Row],[Trial 3]],Table1[[#This Row],[Trial 4]],Table1[[#This Row],[Trial 5]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -714,17 +1867,23 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EB5FE23A-95DE-49E8-A701-F7A11CA11736}" name="Table2" displayName="Table2" ref="A9:G15" totalsRowShown="0" headerRowDxfId="1" dataDxfId="25">
-  <autoFilter ref="A9:G15" xr:uid="{DF255E16-AA76-4E44-9EE2-78CAA550EFC3}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8433774D-B5F6-4C97-A2FE-18CC857D610F}" name="Scenario 2" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{3F3A9BF0-DD6F-42C9-9EAE-09F1AF290E8A}" name="Trail 1" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{6DFEF4BE-4F7F-4715-998F-68F5FF00D87F}" name="Trial 2" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{640A40A4-712D-4AA4-98BC-3BC262190FFD}" name="Trial 3" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{C4754EA0-8815-4DA6-9DA3-0021FD1B3949}" name="Trial 4" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{1A9065D0-EB53-4254-AEBD-1114512F22B9}" name="Trial 5" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{55A6668E-6BC4-4D32-96B7-11634AAE9248}" name="Average" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EB5FE23A-95DE-49E8-A701-F7A11CA11736}" name="Table2" displayName="Table2" ref="A9:I15" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+  <autoFilter ref="A9:I15" xr:uid="{DF255E16-AA76-4E44-9EE2-78CAA550EFC3}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{8433774D-B5F6-4C97-A2FE-18CC857D610F}" name="Scenario 2" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{3F3A9BF0-DD6F-42C9-9EAE-09F1AF290E8A}" name="Trail 1" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{6DFEF4BE-4F7F-4715-998F-68F5FF00D87F}" name="Trial 2" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{640A40A4-712D-4AA4-98BC-3BC262190FFD}" name="Trial 3" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{C4754EA0-8815-4DA6-9DA3-0021FD1B3949}" name="Trial 4" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{1A9065D0-EB53-4254-AEBD-1114512F22B9}" name="Trial 5" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{55A6668E-6BC4-4D32-96B7-11634AAE9248}" name="Average" dataDxfId="10">
       <calculatedColumnFormula>AVERAGE(Table2[[#This Row],[Trail 1]:[Trial 5]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{37B686A6-57DC-4512-8FE0-0D1CE76377AA}" name="Standard Deviation (Sample)" dataDxfId="9">
+      <calculatedColumnFormula>_xlfn.STDEV.S(Table2[[#This Row],[Trail 1]],Table2[[#This Row],[Trial 2]],Table2[[#This Row],[Trial 3]],Table2[[#This Row],[Trial 4]],Table2[[#This Row],[Trial 5]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{E697CADB-6027-4758-A9C7-98F13CD93B4F}" name="Standard Deviation (Population)" dataDxfId="8">
+      <calculatedColumnFormula>_xlfn.STDEV.P(Table2[[#This Row],[Trail 1]],Table2[[#This Row],[Trial 2]],Table2[[#This Row],[Trial 3]],Table2[[#This Row],[Trial 4]],Table2[[#This Row],[Trial 5]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -732,17 +1891,23 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C27265AF-AFE7-4BE5-8C74-418137699BE1}" name="Table3" displayName="Table3" ref="A17:G23" totalsRowShown="0" headerRowDxfId="2" dataDxfId="10">
-  <autoFilter ref="A17:G23" xr:uid="{9564998E-8F11-4F8F-961E-B5FC9E7B6C69}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{55259A19-EA47-4FD5-B9FD-2DF4961E769C}" name="Scenario 3" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{A49B3B5C-E159-41BB-ADBC-1CB720664984}" name="Trail 1" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{6EF104E1-E465-4735-B17F-BC06FAA41212}" name="Trial 2" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{8DEE7FFF-26A7-4F7A-A6AF-84336ADF47D1}" name="Trial 3" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{815CFBCB-DFE4-4D65-8461-BC1BA8CE7982}" name="Trial 4" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{5C82AED9-720B-4A95-B0C0-6FF20997793D}" name="Trial 5" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{EC98BBC9-8B37-4EE3-9A7B-9E2217CEB3C2}" name="Average" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C27265AF-AFE7-4BE5-8C74-418137699BE1}" name="Table3" displayName="Table3" ref="A17:I23" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+  <autoFilter ref="A17:I23" xr:uid="{9564998E-8F11-4F8F-961E-B5FC9E7B6C69}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{55259A19-EA47-4FD5-B9FD-2DF4961E769C}" name="Scenario 3" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{A49B3B5C-E159-41BB-ADBC-1CB720664984}" name="Trail 1" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{6EF104E1-E465-4735-B17F-BC06FAA41212}" name="Trial 2" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{8DEE7FFF-26A7-4F7A-A6AF-84336ADF47D1}" name="Trial 3" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{815CFBCB-DFE4-4D65-8461-BC1BA8CE7982}" name="Trial 4" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{5C82AED9-720B-4A95-B0C0-6FF20997793D}" name="Trial 5" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{EC98BBC9-8B37-4EE3-9A7B-9E2217CEB3C2}" name="Average" dataDxfId="2">
       <calculatedColumnFormula>AVERAGE(Table3[[#This Row],[Trail 1]:[Trial 5]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{E9B183DF-E08B-42D2-AA6F-769A10AC75C2}" name="Standard Deviation (Sample)" dataDxfId="1">
+      <calculatedColumnFormula>_xlfn.STDEV.S(Table3[[#This Row],[Trail 1]],Table3[[#This Row],[Trial 2]],Table3[[#This Row],[Trial 3]],Table3[[#This Row],[Trial 4]],Table3[[#This Row],[Trial 5]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{E192697A-CEBE-478C-BE9A-A1282A216304}" name="Standard Deviation (Population)" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.STDEV.P(Table3[[#This Row],[Trail 1]],Table3[[#This Row],[Trial 2]],Table3[[#This Row],[Trial 3]],Table3[[#This Row],[Trial 4]],Table3[[#This Row],[Trial 5]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1046,10 +2211,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C467ECE-ABB1-40A2-AABC-778C2CF7EEBD}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1057,10 +2222,12 @@
     <col min="1" max="1" width="37.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -1082,493 +2249,682 @@
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="5">
         <v>77</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="5">
         <v>73</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="5">
         <v>89</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="5">
         <v>70</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="5">
         <v>71</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="5">
         <f>AVERAGE(Table1[[#This Row],[Trail 1]:[Trial 5]])</f>
         <v>76</v>
       </c>
+      <c r="H2" s="5">
+        <f>_xlfn.STDEV.S(Table1[[#This Row],[Trail 1]],Table1[[#This Row],[Trial 2]],Table1[[#This Row],[Trial 3]],Table1[[#This Row],[Trial 4]],Table1[[#This Row],[Trial 5]])</f>
+        <v>7.745966692414834</v>
+      </c>
+      <c r="I2" s="5">
+        <f>_xlfn.STDEV.P(Table1[[#This Row],[Trail 1]],Table1[[#This Row],[Trial 2]],Table1[[#This Row],[Trial 3]],Table1[[#This Row],[Trial 4]],Table1[[#This Row],[Trial 5]])</f>
+        <v>6.9282032302755088</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="5">
         <v>34.299999999999997</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="5">
         <v>45.09</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="5">
         <v>34.32</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="5">
         <v>38.33</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="5">
         <v>33.49</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="5">
         <f>AVERAGE(Table1[[#This Row],[Trail 1]:[Trial 5]])</f>
         <v>37.106000000000009</v>
       </c>
+      <c r="H3" s="5">
+        <f>_xlfn.STDEV.S(Table1[[#This Row],[Trail 1]],Table1[[#This Row],[Trial 2]],Table1[[#This Row],[Trial 3]],Table1[[#This Row],[Trial 4]],Table1[[#This Row],[Trial 5]])</f>
+        <v>4.8464760393505975</v>
+      </c>
+      <c r="I3" s="5">
+        <f>_xlfn.STDEV.P(Table1[[#This Row],[Trail 1]],Table1[[#This Row],[Trial 2]],Table1[[#This Row],[Trial 3]],Table1[[#This Row],[Trial 4]],Table1[[#This Row],[Trial 5]])</f>
+        <v>4.3348199501247482</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="5">
         <v>6.74</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="5">
         <v>7.38</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="5">
         <v>7.2</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="5">
         <v>6.09</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="5">
         <v>8.56</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="5">
         <f>AVERAGE(Table1[[#This Row],[Trail 1]:[Trial 5]])</f>
         <v>7.194</v>
       </c>
+      <c r="H4" s="5">
+        <f>_xlfn.STDEV.S(Table1[[#This Row],[Trail 1]],Table1[[#This Row],[Trial 2]],Table1[[#This Row],[Trial 3]],Table1[[#This Row],[Trial 4]],Table1[[#This Row],[Trial 5]])</f>
+        <v>0.91180041675797119</v>
+      </c>
+      <c r="I4" s="5">
+        <f>_xlfn.STDEV.P(Table1[[#This Row],[Trail 1]],Table1[[#This Row],[Trial 2]],Table1[[#This Row],[Trial 3]],Table1[[#This Row],[Trial 4]],Table1[[#This Row],[Trial 5]])</f>
+        <v>0.81553908551338061</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="5">
         <v>9.44</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="5">
         <v>7.76</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="5">
         <v>8.7100000000000009</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="5">
         <v>7.33</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="5">
         <v>7.27</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="5">
         <f>AVERAGE(Table1[[#This Row],[Trail 1]:[Trial 5]])</f>
         <v>8.1020000000000003</v>
       </c>
+      <c r="H5" s="5">
+        <f>_xlfn.STDEV.S(Table1[[#This Row],[Trail 1]],Table1[[#This Row],[Trial 2]],Table1[[#This Row],[Trial 3]],Table1[[#This Row],[Trial 4]],Table1[[#This Row],[Trial 5]])</f>
+        <v>0.94407097190835798</v>
+      </c>
+      <c r="I5" s="5">
+        <f>_xlfn.STDEV.P(Table1[[#This Row],[Trail 1]],Table1[[#This Row],[Trial 2]],Table1[[#This Row],[Trial 3]],Table1[[#This Row],[Trial 4]],Table1[[#This Row],[Trial 5]])</f>
+        <v>0.84440274750855038</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="5">
         <v>8.74</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="5">
         <v>10.86</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="5">
         <v>7.72</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="5">
         <v>9.94</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="5">
         <v>7.15</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="5">
         <f>AVERAGE(Table1[[#This Row],[Trail 1]:[Trial 5]])</f>
         <v>8.8819999999999997</v>
       </c>
+      <c r="H6" s="5">
+        <f>_xlfn.STDEV.S(Table1[[#This Row],[Trail 1]],Table1[[#This Row],[Trial 2]],Table1[[#This Row],[Trial 3]],Table1[[#This Row],[Trial 4]],Table1[[#This Row],[Trial 5]])</f>
+        <v>1.5331405675932013</v>
+      </c>
+      <c r="I6" s="5">
+        <f>_xlfn.STDEV.P(Table1[[#This Row],[Trail 1]],Table1[[#This Row],[Trial 2]],Table1[[#This Row],[Trial 3]],Table1[[#This Row],[Trial 4]],Table1[[#This Row],[Trial 5]])</f>
+        <v>1.3712826112804044</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="5">
         <v>77.37</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="5">
         <v>116.64</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="5">
         <v>108.44</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="5">
         <v>79.56</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="5">
         <v>78.39</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="5">
         <f>AVERAGE(Table1[[#This Row],[Trail 1]:[Trial 5]])</f>
         <v>92.08</v>
       </c>
+      <c r="H7" s="5">
+        <f>_xlfn.STDEV.S(Table1[[#This Row],[Trail 1]],Table1[[#This Row],[Trial 2]],Table1[[#This Row],[Trial 3]],Table1[[#This Row],[Trial 4]],Table1[[#This Row],[Trial 5]])</f>
+        <v>18.916882671307164</v>
+      </c>
+      <c r="I7" s="5">
+        <f>_xlfn.STDEV.P(Table1[[#This Row],[Trail 1]],Table1[[#This Row],[Trial 2]],Table1[[#This Row],[Trial 3]],Table1[[#This Row],[Trial 4]],Table1[[#This Row],[Trial 5]])</f>
+        <v>16.919774230172269</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="H9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="5">
         <v>141</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="5">
         <v>154</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="5">
         <v>149</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="5">
         <v>150</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="5">
         <v>158</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="5">
         <f>AVERAGE(Table2[[#This Row],[Trail 1]:[Trial 5]])</f>
         <v>150.4</v>
       </c>
+      <c r="H10" s="5">
+        <f>_xlfn.STDEV.S(Table2[[#This Row],[Trail 1]],Table2[[#This Row],[Trial 2]],Table2[[#This Row],[Trial 3]],Table2[[#This Row],[Trial 4]],Table2[[#This Row],[Trial 5]])</f>
+        <v>6.3482280992415516</v>
+      </c>
+      <c r="I10" s="5">
+        <f>_xlfn.STDEV.P(Table2[[#This Row],[Trail 1]],Table2[[#This Row],[Trial 2]],Table2[[#This Row],[Trial 3]],Table2[[#This Row],[Trial 4]],Table2[[#This Row],[Trial 5]])</f>
+        <v>5.6780278266313564</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="5">
         <v>35.03</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="5">
         <v>31.11</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="5">
         <v>27.94</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="5">
         <v>33.29</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="5">
         <v>29.84</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="5">
         <f>AVERAGE(Table2[[#This Row],[Trail 1]:[Trial 5]])</f>
         <v>31.442</v>
       </c>
+      <c r="H11" s="5">
+        <f>_xlfn.STDEV.S(Table2[[#This Row],[Trail 1]],Table2[[#This Row],[Trial 2]],Table2[[#This Row],[Trial 3]],Table2[[#This Row],[Trial 4]],Table2[[#This Row],[Trial 5]])</f>
+        <v>2.7941671388805647</v>
+      </c>
+      <c r="I11" s="5">
+        <f>_xlfn.STDEV.P(Table2[[#This Row],[Trail 1]],Table2[[#This Row],[Trial 2]],Table2[[#This Row],[Trial 3]],Table2[[#This Row],[Trial 4]],Table2[[#This Row],[Trial 5]])</f>
+        <v>2.4991790652132151</v>
+      </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="5">
         <v>14.22</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="5">
         <v>12.23</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="5">
         <v>13.46</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="5">
         <v>11.96</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="5">
         <v>12.34</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="5">
         <f>AVERAGE(Table2[[#This Row],[Trail 1]:[Trial 5]])</f>
         <v>12.842000000000002</v>
       </c>
+      <c r="H12" s="5">
+        <f>_xlfn.STDEV.S(Table2[[#This Row],[Trail 1]],Table2[[#This Row],[Trial 2]],Table2[[#This Row],[Trial 3]],Table2[[#This Row],[Trial 4]],Table2[[#This Row],[Trial 5]])</f>
+        <v>0.95985415558823328</v>
+      </c>
+      <c r="I12" s="5">
+        <f>_xlfn.STDEV.P(Table2[[#This Row],[Trail 1]],Table2[[#This Row],[Trial 2]],Table2[[#This Row],[Trial 3]],Table2[[#This Row],[Trial 4]],Table2[[#This Row],[Trial 5]])</f>
+        <v>0.85851965615237968</v>
+      </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="5">
         <v>17.77</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="5">
         <v>18.18</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="5">
         <v>17.78</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="5">
         <v>17.52</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="5">
         <v>14.27</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="5">
         <f>AVERAGE(Table2[[#This Row],[Trail 1]:[Trial 5]])</f>
         <v>17.103999999999999</v>
       </c>
+      <c r="H13" s="5">
+        <f>_xlfn.STDEV.S(Table2[[#This Row],[Trail 1]],Table2[[#This Row],[Trial 2]],Table2[[#This Row],[Trial 3]],Table2[[#This Row],[Trial 4]],Table2[[#This Row],[Trial 5]])</f>
+        <v>1.6017896241392005</v>
+      </c>
+      <c r="I13" s="5">
+        <f>_xlfn.STDEV.P(Table2[[#This Row],[Trail 1]],Table2[[#This Row],[Trial 2]],Table2[[#This Row],[Trial 3]],Table2[[#This Row],[Trial 4]],Table2[[#This Row],[Trial 5]])</f>
+        <v>1.4326841940916359</v>
+      </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="5">
         <v>16.18</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="5">
         <v>19.829999999999998</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="5">
         <v>17.77</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="5">
         <v>18.170000000000002</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="5">
         <v>19.02</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="5">
         <f>AVERAGE(Table2[[#This Row],[Trail 1]:[Trial 5]])</f>
         <v>18.193999999999999</v>
       </c>
+      <c r="H14" s="5">
+        <f>_xlfn.STDEV.S(Table2[[#This Row],[Trail 1]],Table2[[#This Row],[Trial 2]],Table2[[#This Row],[Trial 3]],Table2[[#This Row],[Trial 4]],Table2[[#This Row],[Trial 5]])</f>
+        <v>1.3779804062467647</v>
+      </c>
+      <c r="I14" s="5">
+        <f>_xlfn.STDEV.P(Table2[[#This Row],[Trail 1]],Table2[[#This Row],[Trial 2]],Table2[[#This Row],[Trial 3]],Table2[[#This Row],[Trial 4]],Table2[[#This Row],[Trial 5]])</f>
+        <v>1.2325031440122167</v>
+      </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="5">
         <v>128.53</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="5">
         <v>117.05</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="5">
         <v>105.81</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="5">
         <v>136.58000000000001</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="5">
         <v>117.38</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="5">
         <f>AVERAGE(Table2[[#This Row],[Trail 1]:[Trial 5]])</f>
         <v>121.07000000000001</v>
       </c>
+      <c r="H15" s="5">
+        <f>_xlfn.STDEV.S(Table2[[#This Row],[Trail 1]],Table2[[#This Row],[Trial 2]],Table2[[#This Row],[Trial 3]],Table2[[#This Row],[Trial 4]],Table2[[#This Row],[Trial 5]])</f>
+        <v>11.820065566654023</v>
+      </c>
+      <c r="I15" s="5">
+        <f>_xlfn.STDEV.P(Table2[[#This Row],[Trail 1]],Table2[[#This Row],[Trial 2]],Table2[[#This Row],[Trial 3]],Table2[[#This Row],[Trial 4]],Table2[[#This Row],[Trial 5]])</f>
+        <v>10.572188042217187</v>
+      </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="H17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="5">
         <v>183</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="5">
         <v>190</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="5">
         <v>185</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="5">
         <v>193</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="5">
         <v>190</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="5">
         <f>AVERAGE(Table3[[#This Row],[Trail 1]:[Trial 5]])</f>
         <v>188.2</v>
       </c>
+      <c r="H18" s="5">
+        <f>_xlfn.STDEV.S(Table3[[#This Row],[Trail 1]],Table3[[#This Row],[Trial 2]],Table3[[#This Row],[Trial 3]],Table3[[#This Row],[Trial 4]],Table3[[#This Row],[Trial 5]])</f>
+        <v>4.0865633483405102</v>
+      </c>
+      <c r="I18" s="5">
+        <f>_xlfn.STDEV.P(Table3[[#This Row],[Trail 1]],Table3[[#This Row],[Trial 2]],Table3[[#This Row],[Trial 3]],Table3[[#This Row],[Trial 4]],Table3[[#This Row],[Trial 5]])</f>
+        <v>3.6551333764994132</v>
+      </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="5">
         <v>28.54</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="5">
         <v>31.12</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="5">
         <v>27.81</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="5">
         <v>30.89</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="5">
         <v>27.27</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="5">
         <f>AVERAGE(Table3[[#This Row],[Trail 1]:[Trial 5]])</f>
         <v>29.125999999999998</v>
       </c>
+      <c r="H19" s="5">
+        <f>_xlfn.STDEV.S(Table3[[#This Row],[Trail 1]],Table3[[#This Row],[Trial 2]],Table3[[#This Row],[Trial 3]],Table3[[#This Row],[Trial 4]],Table3[[#This Row],[Trial 5]])</f>
+        <v>1.7753675675757974</v>
+      </c>
+      <c r="I19" s="5">
+        <f>_xlfn.STDEV.P(Table3[[#This Row],[Trail 1]],Table3[[#This Row],[Trial 2]],Table3[[#This Row],[Trial 3]],Table3[[#This Row],[Trial 4]],Table3[[#This Row],[Trial 5]])</f>
+        <v>1.5879370264591737</v>
+      </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="5">
         <v>19.98</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="5">
         <v>20.5</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="5">
         <v>20.84</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="5">
         <v>20.55</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="5">
         <v>21.69</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="5">
         <f>AVERAGE(Table3[[#This Row],[Trail 1]:[Trial 5]])</f>
         <v>20.712</v>
       </c>
+      <c r="H20" s="5">
+        <f>_xlfn.STDEV.S(Table3[[#This Row],[Trail 1]],Table3[[#This Row],[Trial 2]],Table3[[#This Row],[Trial 3]],Table3[[#This Row],[Trial 4]],Table3[[#This Row],[Trial 5]])</f>
+        <v>0.62846638732711901</v>
+      </c>
+      <c r="I20" s="5">
+        <f>_xlfn.STDEV.P(Table3[[#This Row],[Trail 1]],Table3[[#This Row],[Trial 2]],Table3[[#This Row],[Trial 3]],Table3[[#This Row],[Trial 4]],Table3[[#This Row],[Trial 5]])</f>
+        <v>0.56211742545486021</v>
+      </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="5">
         <v>24.29</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="5">
         <v>26.15</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="5">
         <v>25.07</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="5">
         <v>23.19</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="5">
         <v>23.46</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="5">
         <f>AVERAGE(Table3[[#This Row],[Trail 1]:[Trial 5]])</f>
         <v>24.431999999999999</v>
       </c>
+      <c r="H21" s="5">
+        <f>_xlfn.STDEV.S(Table3[[#This Row],[Trail 1]],Table3[[#This Row],[Trial 2]],Table3[[#This Row],[Trial 3]],Table3[[#This Row],[Trial 4]],Table3[[#This Row],[Trial 5]])</f>
+        <v>1.210999587118013</v>
+      </c>
+      <c r="I21" s="5">
+        <f>_xlfn.STDEV.P(Table3[[#This Row],[Trail 1]],Table3[[#This Row],[Trial 2]],Table3[[#This Row],[Trial 3]],Table3[[#This Row],[Trial 4]],Table3[[#This Row],[Trial 5]])</f>
+        <v>1.0831509590080222</v>
+      </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="5">
         <v>26.73</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="5">
         <v>30.28</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="5">
         <v>27.44</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="5">
         <v>28.46</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="5">
         <v>27.66</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="5">
         <f>AVERAGE(Table3[[#This Row],[Trail 1]:[Trial 5]])</f>
         <v>28.113999999999997</v>
       </c>
+      <c r="H22" s="5">
+        <f>_xlfn.STDEV.S(Table3[[#This Row],[Trail 1]],Table3[[#This Row],[Trial 2]],Table3[[#This Row],[Trial 3]],Table3[[#This Row],[Trial 4]],Table3[[#This Row],[Trial 5]])</f>
+        <v>1.3589628398157179</v>
+      </c>
+      <c r="I22" s="5">
+        <f>_xlfn.STDEV.P(Table3[[#This Row],[Trail 1]],Table3[[#This Row],[Trial 2]],Table3[[#This Row],[Trial 3]],Table3[[#This Row],[Trial 4]],Table3[[#This Row],[Trial 5]])</f>
+        <v>1.2154933154896412</v>
+      </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="5">
         <v>122.71</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="5">
         <v>121.45</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="5">
         <v>127.22</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="5">
         <v>130.29</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="5">
         <v>125.21</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="5">
         <f>AVERAGE(Table3[[#This Row],[Trail 1]:[Trial 5]])</f>
         <v>125.376</v>
+      </c>
+      <c r="H23" s="5">
+        <f>_xlfn.STDEV.S(Table3[[#This Row],[Trail 1]],Table3[[#This Row],[Trial 2]],Table3[[#This Row],[Trial 3]],Table3[[#This Row],[Trial 4]],Table3[[#This Row],[Trial 5]])</f>
+        <v>3.5389376937154435</v>
+      </c>
+      <c r="I23" s="5">
+        <f>_xlfn.STDEV.P(Table3[[#This Row],[Trail 1]],Table3[[#This Row],[Trial 2]],Table3[[#This Row],[Trial 3]],Table3[[#This Row],[Trial 4]],Table3[[#This Row],[Trial 5]])</f>
+        <v>3.1653221005136252</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="3">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1797,18 +3153,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1831,18 +3187,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65693B21-B539-40D5-BC96-EDD8E058BB3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E73B963-DA16-4620-8EA4-B5A29708149E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65693B21-B539-40D5-BC96-EDD8E058BB3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>